<commit_message>
Planung und Zeitplanung überarbeitet
</commit_message>
<xml_diff>
--- a/doc/Zeitplanung.xlsx
+++ b/doc/Zeitplanung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nick_privat\FlappyExtremeProject\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{380E4151-EECC-49C7-8F7B-4C1248A5AEB9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B5850BEB-9763-49D2-B55F-07EB700EC4D8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8376" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplanung" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="58">
   <si>
     <t>Nr.</t>
   </si>
@@ -141,33 +141,6 @@
     <t>Arbeitsjournal nachführen</t>
   </si>
   <si>
-    <t>Anforderung #01</t>
-  </si>
-  <si>
-    <t>Anforderung #02</t>
-  </si>
-  <si>
-    <t>Anforderung #03</t>
-  </si>
-  <si>
-    <t>Anforderung #04</t>
-  </si>
-  <si>
-    <t>Anforderung #05</t>
-  </si>
-  <si>
-    <t>Anforderung #06</t>
-  </si>
-  <si>
-    <t>Anforderung #07</t>
-  </si>
-  <si>
-    <t>Anforderung #08</t>
-  </si>
-  <si>
-    <t>Anforderung #09</t>
-  </si>
-  <si>
     <t>Testfälle erstellen</t>
   </si>
   <si>
@@ -249,10 +222,25 @@
     <t>-</t>
   </si>
   <si>
-    <t>14.12.</t>
-  </si>
-  <si>
-    <t>21.12.</t>
+    <t>#01 Spielfigur Bewegen</t>
+  </si>
+  <si>
+    <t>#02 Hindernisse durchfliegen</t>
+  </si>
+  <si>
+    <t>#03 Hinderniss Counter</t>
+  </si>
+  <si>
+    <t>#04 Nickname eingeben</t>
+  </si>
+  <si>
+    <t>#05 Platzierung Scoreboard</t>
+  </si>
+  <si>
+    <t>#06 Top 10</t>
+  </si>
+  <si>
+    <t>09.01.</t>
   </si>
 </sst>
 </file>
@@ -1100,7 +1088,7 @@
     </xf>
     <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1398,18 +1386,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="16" fontId="11" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="11" fillId="16" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1550,16 +1526,16 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>51</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1618,7 +1594,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
@@ -2131,8 +2107,8 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AS23" sqref="AS23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="W16" sqref="W16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -2253,7 +2229,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="86"/>
       <c r="H3" s="23" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
@@ -2383,7 +2359,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="22"/>
       <c r="H5" s="23" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="I5" s="23"/>
       <c r="J5" s="6"/>
@@ -2451,88 +2427,88 @@
     <row r="7" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="9"/>
       <c r="B7" s="27"/>
-      <c r="C7" s="93" t="s">
+      <c r="C7" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="93"/>
+      <c r="D7" s="90"/>
       <c r="E7" s="28" t="s">
         <v>21</v>
       </c>
       <c r="F7" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="94" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" s="94"/>
-      <c r="I7" s="94"/>
-      <c r="J7" s="94"/>
-      <c r="K7" s="94"/>
-      <c r="L7" s="94"/>
-      <c r="M7" s="95"/>
-      <c r="N7" s="94" t="s">
-        <v>46</v>
-      </c>
-      <c r="O7" s="94"/>
-      <c r="P7" s="94"/>
-      <c r="Q7" s="94"/>
-      <c r="R7" s="94"/>
-      <c r="S7" s="94"/>
-      <c r="T7" s="95"/>
-      <c r="U7" s="94" t="s">
-        <v>47</v>
-      </c>
-      <c r="V7" s="94"/>
-      <c r="W7" s="94"/>
-      <c r="X7" s="94"/>
-      <c r="Y7" s="94"/>
-      <c r="Z7" s="94"/>
-      <c r="AA7" s="95"/>
-      <c r="AB7" s="96" t="s">
-        <v>48</v>
-      </c>
-      <c r="AC7" s="94"/>
-      <c r="AD7" s="94"/>
-      <c r="AE7" s="94"/>
-      <c r="AF7" s="94"/>
-      <c r="AG7" s="94"/>
-      <c r="AH7" s="95"/>
-      <c r="AI7" s="94" t="s">
-        <v>49</v>
-      </c>
-      <c r="AJ7" s="94"/>
-      <c r="AK7" s="94"/>
-      <c r="AL7" s="94"/>
-      <c r="AM7" s="94"/>
-      <c r="AN7" s="94"/>
-      <c r="AO7" s="95"/>
-      <c r="AP7" s="96" t="s">
-        <v>50</v>
-      </c>
-      <c r="AQ7" s="94"/>
-      <c r="AR7" s="94"/>
-      <c r="AS7" s="94"/>
-      <c r="AT7" s="94"/>
-      <c r="AU7" s="94"/>
-      <c r="AV7" s="95"/>
-      <c r="AW7" s="94" t="s">
-        <v>51</v>
-      </c>
-      <c r="AX7" s="94"/>
-      <c r="AY7" s="94"/>
-      <c r="AZ7" s="94"/>
-      <c r="BA7" s="94"/>
-      <c r="BB7" s="94"/>
-      <c r="BC7" s="95"/>
-      <c r="BD7" s="96" t="s">
-        <v>52</v>
-      </c>
-      <c r="BE7" s="94"/>
-      <c r="BF7" s="94"/>
-      <c r="BG7" s="94"/>
-      <c r="BH7" s="94"/>
-      <c r="BI7" s="94"/>
-      <c r="BJ7" s="97"/>
+      <c r="G7" s="91" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="91"/>
+      <c r="I7" s="91"/>
+      <c r="J7" s="91"/>
+      <c r="K7" s="91"/>
+      <c r="L7" s="91"/>
+      <c r="M7" s="92"/>
+      <c r="N7" s="91" t="s">
+        <v>37</v>
+      </c>
+      <c r="O7" s="91"/>
+      <c r="P7" s="91"/>
+      <c r="Q7" s="91"/>
+      <c r="R7" s="91"/>
+      <c r="S7" s="91"/>
+      <c r="T7" s="92"/>
+      <c r="U7" s="91" t="s">
+        <v>38</v>
+      </c>
+      <c r="V7" s="91"/>
+      <c r="W7" s="91"/>
+      <c r="X7" s="91"/>
+      <c r="Y7" s="91"/>
+      <c r="Z7" s="91"/>
+      <c r="AA7" s="92"/>
+      <c r="AB7" s="93" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC7" s="91"/>
+      <c r="AD7" s="91"/>
+      <c r="AE7" s="91"/>
+      <c r="AF7" s="91"/>
+      <c r="AG7" s="91"/>
+      <c r="AH7" s="92"/>
+      <c r="AI7" s="91" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ7" s="91"/>
+      <c r="AK7" s="91"/>
+      <c r="AL7" s="91"/>
+      <c r="AM7" s="91"/>
+      <c r="AN7" s="91"/>
+      <c r="AO7" s="92"/>
+      <c r="AP7" s="93" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ7" s="91"/>
+      <c r="AR7" s="91"/>
+      <c r="AS7" s="91"/>
+      <c r="AT7" s="91"/>
+      <c r="AU7" s="91"/>
+      <c r="AV7" s="92"/>
+      <c r="AW7" s="91" t="s">
+        <v>42</v>
+      </c>
+      <c r="AX7" s="91"/>
+      <c r="AY7" s="91"/>
+      <c r="AZ7" s="91"/>
+      <c r="BA7" s="91"/>
+      <c r="BB7" s="91"/>
+      <c r="BC7" s="92"/>
+      <c r="BD7" s="93" t="s">
+        <v>43</v>
+      </c>
+      <c r="BE7" s="91"/>
+      <c r="BF7" s="91"/>
+      <c r="BG7" s="91"/>
+      <c r="BH7" s="91"/>
+      <c r="BI7" s="91"/>
+      <c r="BJ7" s="94"/>
     </row>
     <row r="8" spans="1:62" ht="45" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="10" t="s">
@@ -2549,7 +2525,7 @@
         <v>4</v>
       </c>
       <c r="F8" s="34" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="G8" s="14" t="s">
         <v>17</v>
@@ -2733,7 +2709,7 @@
       </c>
       <c r="D9" s="42">
         <f>SUM(D10:D13)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" s="32"/>
       <c r="F9" s="31"/>
@@ -2802,14 +2778,14 @@
         <v>12</v>
       </c>
       <c r="C10" s="47" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="D10" s="84"/>
       <c r="E10" s="48">
         <v>1</v>
       </c>
       <c r="F10" s="88" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="G10" s="53"/>
       <c r="H10" s="54"/>
@@ -2834,16 +2810,16 @@
       <c r="AA10" s="58"/>
       <c r="AB10" s="53"/>
       <c r="AC10" s="54"/>
-      <c r="AD10" s="54"/>
-      <c r="AE10" s="54"/>
-      <c r="AF10" s="54"/>
+      <c r="AD10" s="60"/>
+      <c r="AE10" s="60"/>
+      <c r="AF10" s="60"/>
       <c r="AG10" s="57"/>
       <c r="AH10" s="58"/>
       <c r="AI10" s="53"/>
       <c r="AJ10" s="54"/>
-      <c r="AK10" s="54"/>
-      <c r="AL10" s="54"/>
-      <c r="AM10" s="54"/>
+      <c r="AK10" s="60"/>
+      <c r="AL10" s="60"/>
+      <c r="AM10" s="60"/>
       <c r="AN10" s="57"/>
       <c r="AO10" s="58"/>
       <c r="AP10" s="53"/>
@@ -2873,14 +2849,14 @@
         <v>102</v>
       </c>
       <c r="B11" s="44" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C11" s="49">
         <v>4</v>
       </c>
       <c r="D11" s="83">
         <f>SUM(G11:BJ11)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" s="50">
         <v>1</v>
@@ -2891,7 +2867,9 @@
       <c r="I11" s="63">
         <v>1</v>
       </c>
-      <c r="J11" s="63"/>
+      <c r="J11" s="63">
+        <v>1</v>
+      </c>
       <c r="K11" s="85"/>
       <c r="L11" s="62"/>
       <c r="M11" s="58" t="s">
@@ -2915,16 +2893,16 @@
       <c r="AA11" s="58"/>
       <c r="AB11" s="59"/>
       <c r="AC11" s="60"/>
-      <c r="AD11" s="54"/>
-      <c r="AE11" s="54"/>
-      <c r="AF11" s="54"/>
+      <c r="AD11" s="60"/>
+      <c r="AE11" s="60"/>
+      <c r="AF11" s="60"/>
       <c r="AG11" s="57"/>
       <c r="AH11" s="58"/>
       <c r="AI11" s="59"/>
       <c r="AJ11" s="60"/>
-      <c r="AK11" s="54"/>
-      <c r="AL11" s="54"/>
-      <c r="AM11" s="54"/>
+      <c r="AK11" s="60"/>
+      <c r="AL11" s="60"/>
+      <c r="AM11" s="60"/>
       <c r="AN11" s="57"/>
       <c r="AO11" s="58"/>
       <c r="AP11" s="59"/>
@@ -2990,30 +2968,30 @@
       <c r="AA12" s="58"/>
       <c r="AB12" s="59"/>
       <c r="AC12" s="60"/>
-      <c r="AD12" s="54"/>
-      <c r="AE12" s="54"/>
-      <c r="AF12" s="54"/>
+      <c r="AD12" s="60"/>
+      <c r="AE12" s="60"/>
+      <c r="AF12" s="60"/>
       <c r="AG12" s="57"/>
       <c r="AH12" s="58"/>
       <c r="AI12" s="59"/>
       <c r="AJ12" s="60"/>
-      <c r="AK12" s="54"/>
-      <c r="AL12" s="54"/>
-      <c r="AM12" s="54"/>
+      <c r="AK12" s="60"/>
+      <c r="AL12" s="60"/>
+      <c r="AM12" s="60"/>
       <c r="AN12" s="57"/>
       <c r="AO12" s="58"/>
       <c r="AP12" s="59"/>
       <c r="AQ12" s="60"/>
       <c r="AR12" s="61"/>
       <c r="AS12" s="61"/>
-      <c r="AT12" s="55"/>
+      <c r="AT12" s="56"/>
       <c r="AU12" s="57"/>
       <c r="AV12" s="58"/>
       <c r="AW12" s="59"/>
       <c r="AX12" s="60"/>
       <c r="AY12" s="61"/>
       <c r="AZ12" s="61"/>
-      <c r="BA12" s="55"/>
+      <c r="BA12" s="56"/>
       <c r="BB12" s="57"/>
       <c r="BC12" s="58"/>
       <c r="BD12" s="59"/>
@@ -3029,17 +3007,17 @@
         <v>104</v>
       </c>
       <c r="B13" s="44" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C13" s="49" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="D13" s="83"/>
       <c r="E13" s="50">
         <v>1</v>
       </c>
       <c r="F13" s="88" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="G13" s="59"/>
       <c r="H13" s="60"/>
@@ -3064,16 +3042,16 @@
       <c r="AA13" s="67"/>
       <c r="AB13" s="59"/>
       <c r="AC13" s="60"/>
-      <c r="AD13" s="54"/>
-      <c r="AE13" s="54"/>
-      <c r="AF13" s="54"/>
+      <c r="AD13" s="60"/>
+      <c r="AE13" s="60"/>
+      <c r="AF13" s="60"/>
       <c r="AG13" s="66"/>
       <c r="AH13" s="67"/>
       <c r="AI13" s="59"/>
       <c r="AJ13" s="60"/>
-      <c r="AK13" s="54"/>
-      <c r="AL13" s="54"/>
-      <c r="AM13" s="54"/>
+      <c r="AK13" s="60"/>
+      <c r="AL13" s="60"/>
+      <c r="AM13" s="60"/>
       <c r="AN13" s="66"/>
       <c r="AO13" s="67"/>
       <c r="AP13" s="59"/>
@@ -3093,7 +3071,7 @@
       <c r="BD13" s="59"/>
       <c r="BE13" s="60"/>
       <c r="BF13" s="55"/>
-      <c r="BG13" s="61"/>
+      <c r="BG13" s="55"/>
       <c r="BH13" s="55"/>
       <c r="BI13" s="66"/>
       <c r="BJ13" s="67"/>
@@ -3177,7 +3155,7 @@
         <v>201</v>
       </c>
       <c r="B15" s="46" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C15" s="49">
         <v>6</v>
@@ -3188,7 +3166,7 @@
       </c>
       <c r="E15" s="50"/>
       <c r="F15" s="89" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="G15" s="53"/>
       <c r="H15" s="54"/>
@@ -3215,16 +3193,16 @@
       <c r="AA15" s="58"/>
       <c r="AB15" s="53"/>
       <c r="AC15" s="54"/>
-      <c r="AD15" s="54"/>
-      <c r="AE15" s="54"/>
-      <c r="AF15" s="54"/>
+      <c r="AD15" s="60"/>
+      <c r="AE15" s="60"/>
+      <c r="AF15" s="60"/>
       <c r="AG15" s="57"/>
       <c r="AH15" s="58"/>
       <c r="AI15" s="53"/>
       <c r="AJ15" s="54"/>
-      <c r="AK15" s="54"/>
-      <c r="AL15" s="54"/>
-      <c r="AM15" s="54"/>
+      <c r="AK15" s="60"/>
+      <c r="AL15" s="60"/>
+      <c r="AM15" s="60"/>
       <c r="AN15" s="57"/>
       <c r="AO15" s="58"/>
       <c r="AP15" s="53"/>
@@ -3254,7 +3232,7 @@
         <v>202</v>
       </c>
       <c r="B16" s="46" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C16" s="49">
         <v>4</v>
@@ -3288,16 +3266,16 @@
       <c r="AA16" s="58"/>
       <c r="AB16" s="59"/>
       <c r="AC16" s="60"/>
-      <c r="AD16" s="54"/>
-      <c r="AE16" s="54"/>
-      <c r="AF16" s="54"/>
+      <c r="AD16" s="60"/>
+      <c r="AE16" s="60"/>
+      <c r="AF16" s="60"/>
       <c r="AG16" s="57"/>
       <c r="AH16" s="58"/>
       <c r="AI16" s="59"/>
       <c r="AJ16" s="60"/>
-      <c r="AK16" s="54"/>
-      <c r="AL16" s="54"/>
-      <c r="AM16" s="54"/>
+      <c r="AK16" s="60"/>
+      <c r="AL16" s="60"/>
+      <c r="AM16" s="60"/>
       <c r="AN16" s="57"/>
       <c r="AO16" s="58"/>
       <c r="AP16" s="59"/>
@@ -3357,16 +3335,16 @@
       <c r="AA17" s="58"/>
       <c r="AB17" s="69"/>
       <c r="AC17" s="70"/>
-      <c r="AD17" s="54"/>
-      <c r="AE17" s="54"/>
-      <c r="AF17" s="54"/>
+      <c r="AD17" s="60"/>
+      <c r="AE17" s="60"/>
+      <c r="AF17" s="60"/>
       <c r="AG17" s="57"/>
       <c r="AH17" s="58"/>
       <c r="AI17" s="69"/>
       <c r="AJ17" s="70"/>
-      <c r="AK17" s="54"/>
-      <c r="AL17" s="54"/>
-      <c r="AM17" s="54"/>
+      <c r="AK17" s="60"/>
+      <c r="AL17" s="60"/>
+      <c r="AM17" s="60"/>
       <c r="AN17" s="57"/>
       <c r="AO17" s="58"/>
       <c r="AP17" s="69"/>
@@ -3400,7 +3378,7 @@
       </c>
       <c r="C18" s="41">
         <f>SUM(C19:C30)</f>
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
@@ -3470,7 +3448,7 @@
         <v>301</v>
       </c>
       <c r="B19" s="46" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C19" s="49">
         <v>1</v>
@@ -3480,9 +3458,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="50"/>
-      <c r="F19" s="92" t="s">
-        <v>60</v>
-      </c>
+      <c r="F19" s="51"/>
       <c r="G19" s="53"/>
       <c r="H19" s="54"/>
       <c r="I19" s="55"/>
@@ -3493,8 +3469,8 @@
       <c r="N19" s="53"/>
       <c r="O19" s="54"/>
       <c r="P19" s="63"/>
-      <c r="Q19" s="56"/>
-      <c r="R19" s="90"/>
+      <c r="Q19" s="55"/>
+      <c r="R19" s="56"/>
       <c r="S19" s="57"/>
       <c r="T19" s="58"/>
       <c r="U19" s="53"/>
@@ -3506,16 +3482,16 @@
       <c r="AA19" s="58"/>
       <c r="AB19" s="53"/>
       <c r="AC19" s="54"/>
-      <c r="AD19" s="54"/>
-      <c r="AE19" s="54"/>
-      <c r="AF19" s="54"/>
+      <c r="AD19" s="60"/>
+      <c r="AE19" s="60"/>
+      <c r="AF19" s="60"/>
       <c r="AG19" s="57"/>
       <c r="AH19" s="58"/>
       <c r="AI19" s="53"/>
       <c r="AJ19" s="54"/>
-      <c r="AK19" s="54"/>
-      <c r="AL19" s="54"/>
-      <c r="AM19" s="54"/>
+      <c r="AK19" s="60"/>
+      <c r="AL19" s="60"/>
+      <c r="AM19" s="60"/>
       <c r="AN19" s="57"/>
       <c r="AO19" s="58"/>
       <c r="AP19" s="53"/>
@@ -3545,10 +3521,10 @@
         <v>302</v>
       </c>
       <c r="B20" s="46" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C20" s="49">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D20" s="83">
         <f t="shared" ref="D20:D30" si="0">SUM(G20:BJ20)</f>
@@ -3572,23 +3548,23 @@
       <c r="T20" s="58"/>
       <c r="U20" s="59"/>
       <c r="V20" s="60"/>
-      <c r="W20" s="61"/>
-      <c r="X20" s="61"/>
-      <c r="Y20" s="61"/>
+      <c r="W20" s="55"/>
+      <c r="X20" s="55"/>
+      <c r="Y20" s="56"/>
       <c r="Z20" s="57"/>
       <c r="AA20" s="58"/>
       <c r="AB20" s="59"/>
       <c r="AC20" s="60"/>
-      <c r="AD20" s="54"/>
-      <c r="AE20" s="54"/>
-      <c r="AF20" s="54"/>
+      <c r="AD20" s="60"/>
+      <c r="AE20" s="60"/>
+      <c r="AF20" s="60"/>
       <c r="AG20" s="57"/>
       <c r="AH20" s="58"/>
       <c r="AI20" s="59"/>
       <c r="AJ20" s="60"/>
-      <c r="AK20" s="54"/>
-      <c r="AL20" s="54"/>
-      <c r="AM20" s="54"/>
+      <c r="AK20" s="60"/>
+      <c r="AL20" s="60"/>
+      <c r="AM20" s="60"/>
       <c r="AN20" s="57"/>
       <c r="AO20" s="58"/>
       <c r="AP20" s="59"/>
@@ -3618,7 +3594,7 @@
         <v>303</v>
       </c>
       <c r="B21" s="46" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="C21" s="49">
         <v>14</v>
@@ -3627,11 +3603,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E21" s="50">
-        <v>1</v>
-      </c>
-      <c r="F21" s="92" t="s">
-        <v>61</v>
+      <c r="E21" s="50"/>
+      <c r="F21" s="52">
+        <v>21.12</v>
       </c>
       <c r="G21" s="59"/>
       <c r="H21" s="60"/>
@@ -3651,28 +3625,28 @@
       <c r="V21" s="60"/>
       <c r="W21" s="63"/>
       <c r="X21" s="63"/>
-      <c r="Y21" s="90"/>
+      <c r="Y21" s="87"/>
       <c r="Z21" s="57"/>
       <c r="AA21" s="58"/>
       <c r="AB21" s="59"/>
       <c r="AC21" s="60"/>
-      <c r="AD21" s="54"/>
-      <c r="AE21" s="54"/>
-      <c r="AF21" s="54"/>
+      <c r="AD21" s="60"/>
+      <c r="AE21" s="60"/>
+      <c r="AF21" s="60"/>
       <c r="AG21" s="57"/>
       <c r="AH21" s="58"/>
       <c r="AI21" s="59"/>
       <c r="AJ21" s="60"/>
-      <c r="AK21" s="54"/>
-      <c r="AL21" s="54"/>
-      <c r="AM21" s="54"/>
+      <c r="AK21" s="60"/>
+      <c r="AL21" s="60"/>
+      <c r="AM21" s="60"/>
       <c r="AN21" s="57"/>
       <c r="AO21" s="58"/>
       <c r="AP21" s="59"/>
       <c r="AQ21" s="60"/>
       <c r="AR21" s="55"/>
       <c r="AS21" s="55"/>
-      <c r="AT21" s="55"/>
+      <c r="AT21" s="56"/>
       <c r="AU21" s="57"/>
       <c r="AV21" s="58"/>
       <c r="AW21" s="59"/>
@@ -3695,19 +3669,19 @@
         <v>304</v>
       </c>
       <c r="B22" s="46" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="C22" s="49">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D22" s="83">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E22" s="50">
-        <v>1</v>
-      </c>
-      <c r="F22" s="51"/>
+      <c r="E22" s="50"/>
+      <c r="F22" s="51" t="s">
+        <v>57</v>
+      </c>
       <c r="G22" s="59"/>
       <c r="H22" s="60"/>
       <c r="I22" s="55"/>
@@ -3731,29 +3705,29 @@
       <c r="AA22" s="58"/>
       <c r="AB22" s="59"/>
       <c r="AC22" s="60"/>
-      <c r="AD22" s="54"/>
-      <c r="AE22" s="54"/>
-      <c r="AF22" s="54"/>
+      <c r="AD22" s="60"/>
+      <c r="AE22" s="63"/>
+      <c r="AF22" s="63"/>
       <c r="AG22" s="57"/>
       <c r="AH22" s="58"/>
       <c r="AI22" s="59"/>
       <c r="AJ22" s="60"/>
-      <c r="AK22" s="54"/>
-      <c r="AL22" s="54"/>
-      <c r="AM22" s="54"/>
+      <c r="AK22" s="60"/>
+      <c r="AL22" s="60"/>
+      <c r="AM22" s="60"/>
       <c r="AN22" s="57"/>
       <c r="AO22" s="58"/>
       <c r="AP22" s="59"/>
       <c r="AQ22" s="60"/>
-      <c r="AR22" s="55"/>
+      <c r="AR22" s="87"/>
       <c r="AS22" s="55"/>
-      <c r="AT22" s="55"/>
+      <c r="AT22" s="56"/>
       <c r="AU22" s="57"/>
       <c r="AV22" s="58"/>
       <c r="AW22" s="59"/>
       <c r="AX22" s="60"/>
-      <c r="AY22" s="56"/>
-      <c r="AZ22" s="56"/>
+      <c r="AY22" s="55"/>
+      <c r="AZ22" s="55"/>
       <c r="BA22" s="56"/>
       <c r="BB22" s="57"/>
       <c r="BC22" s="58"/>
@@ -3770,19 +3744,19 @@
         <v>305</v>
       </c>
       <c r="B23" s="46" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="C23" s="49">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D23" s="83">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E23" s="50">
-        <v>2</v>
-      </c>
-      <c r="F23" s="51"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="51" t="s">
+        <v>57</v>
+      </c>
       <c r="G23" s="59"/>
       <c r="H23" s="60"/>
       <c r="I23" s="61"/>
@@ -3806,29 +3780,29 @@
       <c r="AA23" s="58"/>
       <c r="AB23" s="59"/>
       <c r="AC23" s="60"/>
-      <c r="AD23" s="63"/>
-      <c r="AE23" s="63"/>
+      <c r="AD23" s="60"/>
+      <c r="AE23" s="60"/>
       <c r="AF23" s="63"/>
-      <c r="AG23" s="57"/>
+      <c r="AG23" s="63"/>
       <c r="AH23" s="58"/>
-      <c r="AI23" s="59"/>
+      <c r="AI23" s="60"/>
       <c r="AJ23" s="60"/>
-      <c r="AK23" s="54"/>
-      <c r="AL23" s="54"/>
-      <c r="AM23" s="54"/>
+      <c r="AK23" s="60"/>
+      <c r="AL23" s="60"/>
+      <c r="AM23" s="60"/>
       <c r="AN23" s="57"/>
       <c r="AO23" s="58"/>
       <c r="AP23" s="59"/>
       <c r="AQ23" s="60"/>
-      <c r="AR23" s="55"/>
-      <c r="AS23" s="55"/>
-      <c r="AT23" s="55"/>
+      <c r="AR23" s="87"/>
+      <c r="AS23" s="61"/>
+      <c r="AT23" s="56"/>
       <c r="AU23" s="57"/>
       <c r="AV23" s="58"/>
       <c r="AW23" s="59"/>
       <c r="AX23" s="60"/>
-      <c r="AY23" s="56"/>
-      <c r="AZ23" s="56"/>
+      <c r="AY23" s="61"/>
+      <c r="AZ23" s="61"/>
       <c r="BA23" s="56"/>
       <c r="BB23" s="57"/>
       <c r="BC23" s="58"/>
@@ -3845,18 +3819,16 @@
         <v>306</v>
       </c>
       <c r="B24" s="46" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="C24" s="49">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D24" s="83">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E24" s="50">
-        <v>2</v>
-      </c>
+      <c r="E24" s="50"/>
       <c r="F24" s="51"/>
       <c r="G24" s="59"/>
       <c r="H24" s="60"/>
@@ -3881,29 +3853,29 @@
       <c r="AA24" s="58"/>
       <c r="AB24" s="59"/>
       <c r="AC24" s="60"/>
-      <c r="AD24" s="54"/>
-      <c r="AE24" s="63"/>
-      <c r="AF24" s="63"/>
+      <c r="AD24" s="60"/>
+      <c r="AE24" s="60"/>
+      <c r="AF24" s="60"/>
       <c r="AG24" s="57"/>
       <c r="AH24" s="58"/>
-      <c r="AI24" s="59"/>
-      <c r="AJ24" s="60"/>
+      <c r="AI24" s="63"/>
+      <c r="AJ24" s="63"/>
       <c r="AK24" s="63"/>
-      <c r="AL24" s="54"/>
-      <c r="AM24" s="54"/>
+      <c r="AL24" s="60"/>
+      <c r="AM24" s="60"/>
       <c r="AN24" s="57"/>
       <c r="AO24" s="58"/>
       <c r="AP24" s="59"/>
       <c r="AQ24" s="60"/>
       <c r="AR24" s="55"/>
       <c r="AS24" s="55"/>
-      <c r="AT24" s="55"/>
+      <c r="AT24" s="56"/>
       <c r="AU24" s="57"/>
       <c r="AV24" s="58"/>
       <c r="AW24" s="59"/>
       <c r="AX24" s="60"/>
-      <c r="AY24" s="56"/>
-      <c r="AZ24" s="56"/>
+      <c r="AY24" s="55"/>
+      <c r="AZ24" s="55"/>
       <c r="BA24" s="56"/>
       <c r="BB24" s="57"/>
       <c r="BC24" s="58"/>
@@ -3920,14 +3892,16 @@
         <v>307</v>
       </c>
       <c r="B25" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="C25" s="49"/>
+        <v>55</v>
+      </c>
+      <c r="C25" s="49">
+        <v>8</v>
+      </c>
       <c r="D25" s="83">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E25" s="91"/>
+      <c r="E25" s="50"/>
       <c r="F25" s="51"/>
       <c r="G25" s="59"/>
       <c r="H25" s="60"/>
@@ -3952,31 +3926,31 @@
       <c r="AA25" s="58"/>
       <c r="AB25" s="59"/>
       <c r="AC25" s="60"/>
-      <c r="AD25" s="54"/>
-      <c r="AE25" s="54"/>
-      <c r="AF25" s="54"/>
+      <c r="AD25" s="60"/>
+      <c r="AE25" s="60"/>
+      <c r="AF25" s="60"/>
       <c r="AG25" s="57"/>
       <c r="AH25" s="58"/>
-      <c r="AI25" s="59"/>
-      <c r="AJ25" s="60"/>
-      <c r="AK25" s="54"/>
-      <c r="AL25" s="54"/>
-      <c r="AM25" s="54"/>
+      <c r="AI25" s="63"/>
+      <c r="AJ25" s="63"/>
+      <c r="AK25" s="63"/>
+      <c r="AL25" s="60"/>
+      <c r="AM25" s="60"/>
       <c r="AN25" s="57"/>
       <c r="AO25" s="58"/>
       <c r="AP25" s="59"/>
       <c r="AQ25" s="60"/>
       <c r="AR25" s="55"/>
       <c r="AS25" s="55"/>
-      <c r="AT25" s="55"/>
-      <c r="AU25" s="58"/>
+      <c r="AT25" s="56"/>
+      <c r="AU25" s="57"/>
       <c r="AV25" s="58"/>
       <c r="AW25" s="59"/>
       <c r="AX25" s="60"/>
-      <c r="AY25" s="56"/>
-      <c r="AZ25" s="56"/>
+      <c r="AY25" s="55"/>
+      <c r="AZ25" s="55"/>
       <c r="BA25" s="56"/>
-      <c r="BB25" s="58"/>
+      <c r="BB25" s="57"/>
       <c r="BC25" s="58"/>
       <c r="BD25" s="59"/>
       <c r="BE25" s="60"/>
@@ -3991,9 +3965,11 @@
         <v>308</v>
       </c>
       <c r="B26" s="46" t="s">
-        <v>29</v>
-      </c>
-      <c r="C26" s="49"/>
+        <v>56</v>
+      </c>
+      <c r="C26" s="49">
+        <v>4</v>
+      </c>
       <c r="D26" s="83">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4023,16 +3999,16 @@
       <c r="AA26" s="58"/>
       <c r="AB26" s="59"/>
       <c r="AC26" s="60"/>
-      <c r="AD26" s="54"/>
-      <c r="AE26" s="54"/>
-      <c r="AF26" s="54"/>
+      <c r="AD26" s="60"/>
+      <c r="AE26" s="60"/>
+      <c r="AF26" s="60"/>
       <c r="AG26" s="57"/>
       <c r="AH26" s="58"/>
-      <c r="AI26" s="59"/>
-      <c r="AJ26" s="60"/>
-      <c r="AK26" s="54"/>
-      <c r="AL26" s="54"/>
-      <c r="AM26" s="54"/>
+      <c r="AI26" s="63"/>
+      <c r="AJ26" s="63"/>
+      <c r="AK26" s="63"/>
+      <c r="AL26" s="60"/>
+      <c r="AM26" s="60"/>
       <c r="AN26" s="57"/>
       <c r="AO26" s="58"/>
       <c r="AP26" s="59"/>
@@ -4061,9 +4037,7 @@
       <c r="A27" s="12">
         <v>309</v>
       </c>
-      <c r="B27" s="46" t="s">
-        <v>30</v>
-      </c>
+      <c r="B27" s="46"/>
       <c r="C27" s="49"/>
       <c r="D27" s="83">
         <f t="shared" si="0"/>
@@ -4094,16 +4068,16 @@
       <c r="AA27" s="58"/>
       <c r="AB27" s="59"/>
       <c r="AC27" s="60"/>
-      <c r="AD27" s="54"/>
-      <c r="AE27" s="54"/>
-      <c r="AF27" s="54"/>
+      <c r="AD27" s="60"/>
+      <c r="AE27" s="60"/>
+      <c r="AF27" s="60"/>
       <c r="AG27" s="57"/>
       <c r="AH27" s="58"/>
-      <c r="AI27" s="59"/>
+      <c r="AI27" s="60"/>
       <c r="AJ27" s="60"/>
-      <c r="AK27" s="54"/>
-      <c r="AL27" s="54"/>
-      <c r="AM27" s="54"/>
+      <c r="AK27" s="60"/>
+      <c r="AL27" s="60"/>
+      <c r="AM27" s="60"/>
       <c r="AN27" s="57"/>
       <c r="AO27" s="58"/>
       <c r="AP27" s="59"/>
@@ -4132,9 +4106,7 @@
       <c r="A28" s="12">
         <v>310</v>
       </c>
-      <c r="B28" s="46" t="s">
-        <v>31</v>
-      </c>
+      <c r="B28" s="46"/>
       <c r="C28" s="49"/>
       <c r="D28" s="83">
         <f t="shared" si="0"/>
@@ -4165,16 +4137,16 @@
       <c r="AA28" s="58"/>
       <c r="AB28" s="59"/>
       <c r="AC28" s="60"/>
-      <c r="AD28" s="54"/>
-      <c r="AE28" s="54"/>
-      <c r="AF28" s="54"/>
+      <c r="AD28" s="60"/>
+      <c r="AE28" s="60"/>
+      <c r="AF28" s="60"/>
       <c r="AG28" s="57"/>
       <c r="AH28" s="58"/>
       <c r="AI28" s="59"/>
       <c r="AJ28" s="60"/>
-      <c r="AK28" s="54"/>
-      <c r="AL28" s="54"/>
-      <c r="AM28" s="54"/>
+      <c r="AK28" s="60"/>
+      <c r="AL28" s="60"/>
+      <c r="AM28" s="60"/>
       <c r="AN28" s="57"/>
       <c r="AO28" s="58"/>
       <c r="AP28" s="59"/>
@@ -4203,9 +4175,7 @@
       <c r="A29" s="12">
         <v>311</v>
       </c>
-      <c r="B29" s="46" t="s">
-        <v>32</v>
-      </c>
+      <c r="B29" s="46"/>
       <c r="C29" s="49"/>
       <c r="D29" s="83">
         <f t="shared" si="0"/>
@@ -4236,16 +4206,16 @@
       <c r="AA29" s="58"/>
       <c r="AB29" s="71"/>
       <c r="AC29" s="72"/>
-      <c r="AD29" s="54"/>
-      <c r="AE29" s="54"/>
-      <c r="AF29" s="54"/>
+      <c r="AD29" s="60"/>
+      <c r="AE29" s="60"/>
+      <c r="AF29" s="60"/>
       <c r="AG29" s="57"/>
       <c r="AH29" s="58"/>
       <c r="AI29" s="71"/>
       <c r="AJ29" s="72"/>
-      <c r="AK29" s="54"/>
-      <c r="AL29" s="54"/>
-      <c r="AM29" s="54"/>
+      <c r="AK29" s="60"/>
+      <c r="AL29" s="60"/>
+      <c r="AM29" s="60"/>
       <c r="AN29" s="57"/>
       <c r="AO29" s="58"/>
       <c r="AP29" s="71"/>
@@ -4305,16 +4275,16 @@
       <c r="AA30" s="58"/>
       <c r="AB30" s="69"/>
       <c r="AC30" s="70"/>
-      <c r="AD30" s="54"/>
-      <c r="AE30" s="54"/>
-      <c r="AF30" s="54"/>
+      <c r="AD30" s="60"/>
+      <c r="AE30" s="60"/>
+      <c r="AF30" s="60"/>
       <c r="AG30" s="57"/>
       <c r="AH30" s="58"/>
       <c r="AI30" s="69"/>
       <c r="AJ30" s="70"/>
-      <c r="AK30" s="54"/>
-      <c r="AL30" s="54"/>
-      <c r="AM30" s="54"/>
+      <c r="AK30" s="60"/>
+      <c r="AL30" s="60"/>
+      <c r="AM30" s="60"/>
       <c r="AN30" s="57"/>
       <c r="AO30" s="58"/>
       <c r="AP30" s="69"/>
@@ -4418,7 +4388,7 @@
         <v>401</v>
       </c>
       <c r="B32" s="46" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C32" s="49">
         <v>2</v>
@@ -4452,29 +4422,29 @@
       <c r="AA32" s="58"/>
       <c r="AB32" s="53"/>
       <c r="AC32" s="54"/>
-      <c r="AD32" s="55"/>
-      <c r="AE32" s="55"/>
-      <c r="AF32" s="56"/>
+      <c r="AD32" s="60"/>
+      <c r="AE32" s="60"/>
+      <c r="AF32" s="60"/>
       <c r="AG32" s="57"/>
       <c r="AH32" s="58"/>
       <c r="AI32" s="53"/>
       <c r="AJ32" s="54"/>
-      <c r="AK32" s="55"/>
-      <c r="AL32" s="63"/>
-      <c r="AM32" s="55"/>
+      <c r="AK32" s="63"/>
+      <c r="AL32" s="60"/>
+      <c r="AM32" s="60"/>
       <c r="AN32" s="57"/>
       <c r="AO32" s="58"/>
       <c r="AP32" s="53"/>
       <c r="AQ32" s="54"/>
-      <c r="AR32" s="56"/>
+      <c r="AR32" s="55"/>
       <c r="AS32" s="55"/>
       <c r="AT32" s="56"/>
       <c r="AU32" s="57"/>
       <c r="AV32" s="58"/>
       <c r="AW32" s="53"/>
       <c r="AX32" s="54"/>
-      <c r="AY32" s="56"/>
-      <c r="AZ32" s="56"/>
+      <c r="AY32" s="55"/>
+      <c r="AZ32" s="55"/>
       <c r="BA32" s="56"/>
       <c r="BB32" s="57"/>
       <c r="BC32" s="58"/>
@@ -4491,7 +4461,7 @@
         <v>402</v>
       </c>
       <c r="B33" s="46" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C33" s="49">
         <v>2</v>
@@ -4525,29 +4495,29 @@
       <c r="AA33" s="58"/>
       <c r="AB33" s="59"/>
       <c r="AC33" s="60"/>
-      <c r="AD33" s="55"/>
-      <c r="AE33" s="55"/>
-      <c r="AF33" s="56"/>
+      <c r="AD33" s="60"/>
+      <c r="AE33" s="60"/>
+      <c r="AF33" s="60"/>
       <c r="AG33" s="57"/>
       <c r="AH33" s="58"/>
       <c r="AI33" s="59"/>
       <c r="AJ33" s="60"/>
-      <c r="AK33" s="55"/>
+      <c r="AK33" s="60"/>
       <c r="AL33" s="63"/>
-      <c r="AM33" s="56"/>
+      <c r="AM33" s="63"/>
       <c r="AN33" s="57"/>
       <c r="AO33" s="58"/>
       <c r="AP33" s="59"/>
       <c r="AQ33" s="60"/>
-      <c r="AR33" s="56"/>
+      <c r="AR33" s="55"/>
       <c r="AS33" s="55"/>
       <c r="AT33" s="56"/>
       <c r="AU33" s="57"/>
       <c r="AV33" s="58"/>
       <c r="AW33" s="59"/>
       <c r="AX33" s="60"/>
-      <c r="AY33" s="56"/>
-      <c r="AZ33" s="56"/>
+      <c r="AY33" s="55"/>
+      <c r="AZ33" s="55"/>
       <c r="BA33" s="56"/>
       <c r="BB33" s="57"/>
       <c r="BC33" s="58"/>
@@ -4564,7 +4534,7 @@
         <v>403</v>
       </c>
       <c r="B34" s="46" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C34" s="49">
         <v>8</v>
@@ -4598,29 +4568,29 @@
       <c r="AA34" s="58"/>
       <c r="AB34" s="59"/>
       <c r="AC34" s="60"/>
-      <c r="AD34" s="55"/>
-      <c r="AE34" s="55"/>
-      <c r="AF34" s="56"/>
+      <c r="AD34" s="60"/>
+      <c r="AE34" s="60"/>
+      <c r="AF34" s="60"/>
       <c r="AG34" s="57"/>
       <c r="AH34" s="58"/>
       <c r="AI34" s="59"/>
       <c r="AJ34" s="60"/>
-      <c r="AK34" s="55"/>
+      <c r="AK34" s="60"/>
       <c r="AL34" s="63"/>
       <c r="AM34" s="63"/>
       <c r="AN34" s="57"/>
       <c r="AO34" s="58"/>
       <c r="AP34" s="59"/>
       <c r="AQ34" s="60"/>
-      <c r="AR34" s="56"/>
+      <c r="AR34" s="55"/>
       <c r="AS34" s="55"/>
       <c r="AT34" s="56"/>
       <c r="AU34" s="57"/>
       <c r="AV34" s="58"/>
       <c r="AW34" s="59"/>
       <c r="AX34" s="60"/>
-      <c r="AY34" s="56"/>
-      <c r="AZ34" s="56"/>
+      <c r="AY34" s="55"/>
+      <c r="AZ34" s="55"/>
       <c r="BA34" s="56"/>
       <c r="BB34" s="57"/>
       <c r="BC34" s="58"/>
@@ -4667,16 +4637,16 @@
       <c r="AA35" s="58"/>
       <c r="AB35" s="69"/>
       <c r="AC35" s="70"/>
-      <c r="AD35" s="55"/>
-      <c r="AE35" s="55"/>
-      <c r="AF35" s="56"/>
+      <c r="AD35" s="60"/>
+      <c r="AE35" s="60"/>
+      <c r="AF35" s="60"/>
       <c r="AG35" s="57"/>
       <c r="AH35" s="58"/>
       <c r="AI35" s="69"/>
       <c r="AJ35" s="70"/>
-      <c r="AK35" s="55"/>
-      <c r="AL35" s="55"/>
-      <c r="AM35" s="56"/>
+      <c r="AK35" s="60"/>
+      <c r="AL35" s="60"/>
+      <c r="AM35" s="60"/>
       <c r="AN35" s="57"/>
       <c r="AO35" s="58"/>
       <c r="AP35" s="69"/>
@@ -4710,7 +4680,7 @@
       </c>
       <c r="C36" s="41">
         <f>SUM(C37:C38)</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D36" s="42">
         <f>SUM(D37:D38)</f>
@@ -4780,11 +4750,9 @@
         <v>501</v>
       </c>
       <c r="B37" s="46" t="s">
-        <v>36</v>
-      </c>
-      <c r="C37" s="49">
-        <v>16</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C37" s="49"/>
       <c r="D37" s="83">
         <f>SUM(G37:BJ37)</f>
         <v>0</v>
@@ -4812,20 +4780,20 @@
       <c r="Y37" s="56"/>
       <c r="Z37" s="57"/>
       <c r="AA37" s="58"/>
-      <c r="AB37" s="63"/>
-      <c r="AC37" s="63"/>
-      <c r="AD37" s="63"/>
-      <c r="AE37" s="63"/>
-      <c r="AF37" s="63"/>
-      <c r="AG37" s="63"/>
-      <c r="AH37" s="63"/>
-      <c r="AI37" s="63"/>
-      <c r="AJ37" s="63"/>
-      <c r="AK37" s="63"/>
-      <c r="AL37" s="63"/>
-      <c r="AM37" s="63"/>
-      <c r="AN37" s="63"/>
-      <c r="AO37" s="63"/>
+      <c r="AB37" s="53"/>
+      <c r="AC37" s="54"/>
+      <c r="AD37" s="60"/>
+      <c r="AE37" s="60"/>
+      <c r="AF37" s="60"/>
+      <c r="AG37" s="57"/>
+      <c r="AH37" s="58"/>
+      <c r="AI37" s="53"/>
+      <c r="AJ37" s="54"/>
+      <c r="AK37" s="60"/>
+      <c r="AL37" s="60"/>
+      <c r="AM37" s="60"/>
+      <c r="AN37" s="57"/>
+      <c r="AO37" s="58"/>
       <c r="AP37" s="53"/>
       <c r="AQ37" s="54"/>
       <c r="AR37" s="55"/>
@@ -4883,16 +4851,16 @@
       <c r="AA38" s="58"/>
       <c r="AB38" s="69"/>
       <c r="AC38" s="70"/>
-      <c r="AD38" s="55"/>
-      <c r="AE38" s="55"/>
-      <c r="AF38" s="56"/>
+      <c r="AD38" s="60"/>
+      <c r="AE38" s="60"/>
+      <c r="AF38" s="60"/>
       <c r="AG38" s="57"/>
       <c r="AH38" s="58"/>
       <c r="AI38" s="69"/>
       <c r="AJ38" s="70"/>
-      <c r="AK38" s="55"/>
-      <c r="AL38" s="55"/>
-      <c r="AM38" s="56"/>
+      <c r="AK38" s="60"/>
+      <c r="AL38" s="60"/>
+      <c r="AM38" s="60"/>
       <c r="AN38" s="57"/>
       <c r="AO38" s="58"/>
       <c r="AP38" s="69"/>
@@ -4926,7 +4894,7 @@
       </c>
       <c r="C39" s="41">
         <f>SUM(C40:C42)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D39" s="42">
         <f>SUM(D40:D42)</f>
@@ -4996,7 +4964,7 @@
         <v>601</v>
       </c>
       <c r="B40" s="46" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C40" s="49">
         <v>2</v>
@@ -5030,16 +4998,16 @@
       <c r="AA40" s="58"/>
       <c r="AB40" s="53"/>
       <c r="AC40" s="54"/>
-      <c r="AD40" s="55"/>
-      <c r="AE40" s="55"/>
-      <c r="AF40" s="56"/>
+      <c r="AD40" s="60"/>
+      <c r="AE40" s="60"/>
+      <c r="AF40" s="60"/>
       <c r="AG40" s="57"/>
       <c r="AH40" s="58"/>
       <c r="AI40" s="53"/>
       <c r="AJ40" s="54"/>
-      <c r="AK40" s="55"/>
-      <c r="AL40" s="55"/>
-      <c r="AM40" s="56"/>
+      <c r="AK40" s="60"/>
+      <c r="AL40" s="60"/>
+      <c r="AM40" s="60"/>
       <c r="AN40" s="57"/>
       <c r="AO40" s="58"/>
       <c r="AP40" s="53"/>
@@ -5069,10 +5037,10 @@
         <v>602</v>
       </c>
       <c r="B41" s="46" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C41" s="49">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D41" s="83">
         <f t="shared" ref="D41:D42" si="2">SUM(G41:BJ41)</f>
@@ -5103,16 +5071,16 @@
       <c r="AA41" s="58"/>
       <c r="AB41" s="59"/>
       <c r="AC41" s="60"/>
-      <c r="AD41" s="55"/>
-      <c r="AE41" s="55"/>
-      <c r="AF41" s="56"/>
+      <c r="AD41" s="60"/>
+      <c r="AE41" s="60"/>
+      <c r="AF41" s="60"/>
       <c r="AG41" s="57"/>
       <c r="AH41" s="58"/>
       <c r="AI41" s="59"/>
       <c r="AJ41" s="60"/>
-      <c r="AK41" s="55"/>
-      <c r="AL41" s="55"/>
-      <c r="AM41" s="56"/>
+      <c r="AK41" s="60"/>
+      <c r="AL41" s="60"/>
+      <c r="AM41" s="60"/>
       <c r="AN41" s="57"/>
       <c r="AO41" s="58"/>
       <c r="AP41" s="59"/>
@@ -5172,16 +5140,16 @@
       <c r="AA42" s="58"/>
       <c r="AB42" s="69"/>
       <c r="AC42" s="70"/>
-      <c r="AD42" s="55"/>
-      <c r="AE42" s="55"/>
-      <c r="AF42" s="56"/>
+      <c r="AD42" s="60"/>
+      <c r="AE42" s="60"/>
+      <c r="AF42" s="60"/>
       <c r="AG42" s="57"/>
       <c r="AH42" s="58"/>
       <c r="AI42" s="69"/>
       <c r="AJ42" s="70"/>
-      <c r="AK42" s="55"/>
-      <c r="AL42" s="55"/>
-      <c r="AM42" s="56"/>
+      <c r="AK42" s="60"/>
+      <c r="AL42" s="60"/>
+      <c r="AM42" s="60"/>
       <c r="AN42" s="57"/>
       <c r="AO42" s="58"/>
       <c r="AP42" s="69"/>
@@ -5213,11 +5181,11 @@
       </c>
       <c r="C43" s="37">
         <f>C39+C36+C31+C18+C14+C9</f>
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5235,7 +5203,7 @@
       </c>
       <c r="J43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K43" s="39">
         <f t="shared" si="3"/>
@@ -5492,10 +5460,10 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="97" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="101"/>
+      <c r="B2" s="98"/>
       <c r="C2" s="79" t="s">
         <v>14</v>
       </c>
@@ -5504,28 +5472,28 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="98" t="str">
+      <c r="A3" s="95" t="str">
         <f>Zeitplanung!B9</f>
         <v>Administration, Planung</v>
       </c>
-      <c r="B3" s="99"/>
+      <c r="B3" s="96"/>
       <c r="C3" s="80">
         <f>Zeitplanung!C9</f>
         <v>9</v>
       </c>
       <c r="D3" s="80">
         <f>Zeitplanung!D9</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" s="82"/>
       <c r="F3" s="81"/>
     </row>
     <row r="4" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="98" t="str">
+      <c r="A4" s="95" t="str">
         <f>Zeitplanung!B14</f>
         <v>Analyse &amp; Design</v>
       </c>
-      <c r="B4" s="99"/>
+      <c r="B4" s="96"/>
       <c r="C4" s="80">
         <f>Zeitplanung!C14</f>
         <v>10</v>
@@ -5538,14 +5506,14 @@
       <c r="F4" s="81"/>
     </row>
     <row r="5" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="98" t="str">
+      <c r="A5" s="95" t="str">
         <f>Zeitplanung!B18</f>
         <v>Implementation</v>
       </c>
-      <c r="B5" s="99"/>
+      <c r="B5" s="96"/>
       <c r="C5" s="80">
         <f>Zeitplanung!C18</f>
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" s="80">
         <f>Zeitplanung!D18</f>
@@ -5555,11 +5523,11 @@
       <c r="F5" s="81"/>
     </row>
     <row r="6" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="98" t="str">
+      <c r="A6" s="95" t="str">
         <f>Zeitplanung!B31</f>
         <v>Testen</v>
       </c>
-      <c r="B6" s="99"/>
+      <c r="B6" s="96"/>
       <c r="C6" s="80">
         <f>Zeitplanung!C31</f>
         <v>12</v>
@@ -5571,14 +5539,14 @@
       <c r="F6" s="81"/>
     </row>
     <row r="7" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="98" t="str">
+      <c r="A7" s="95" t="str">
         <f>Zeitplanung!B36</f>
         <v>Diverses</v>
       </c>
-      <c r="B7" s="99"/>
+      <c r="B7" s="96"/>
       <c r="C7" s="80">
         <f>Zeitplanung!C36</f>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D7" s="80">
         <f>Zeitplanung!D36</f>
@@ -5587,14 +5555,14 @@
       <c r="F7" s="81"/>
     </row>
     <row r="8" spans="1:6" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="98" t="str">
+      <c r="A8" s="95" t="str">
         <f>Zeitplanung!B39</f>
         <v>Abschluss</v>
       </c>
-      <c r="B8" s="99"/>
+      <c r="B8" s="96"/>
       <c r="C8" s="80">
         <f>Zeitplanung!C39</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D8" s="80">
         <f>Zeitplanung!D39</f>

</xml_diff>

<commit_message>
Zeit von Freitag nach getragen
</commit_message>
<xml_diff>
--- a/doc/Zeitplanung.xlsx
+++ b/doc/Zeitplanung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nick_privat\FlappyExtremeProject\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{28B980DC-3175-4D73-83B6-391D91551C0D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{545EAEA5-074D-4DEB-AD75-545F9FFA590A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1594,13 +1594,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2107,8 +2107,8 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -2709,7 +2709,7 @@
       </c>
       <c r="D9" s="42">
         <f>SUM(D10:D13)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E9" s="32"/>
       <c r="F9" s="31"/>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="D12" s="83">
         <f>SUM(G12:BJ12)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="50">
         <v>1</v>
@@ -2949,7 +2949,9 @@
       <c r="H12" s="60"/>
       <c r="I12" s="61"/>
       <c r="J12" s="61"/>
-      <c r="K12" s="63"/>
+      <c r="K12" s="63">
+        <v>1</v>
+      </c>
       <c r="L12" s="57"/>
       <c r="M12" s="58"/>
       <c r="N12" s="59"/>
@@ -3089,7 +3091,7 @@
       </c>
       <c r="D14" s="42">
         <f>SUM(D15:D17)</f>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E14" s="32"/>
       <c r="F14" s="31"/>
@@ -3241,7 +3243,7 @@
       </c>
       <c r="D16" s="83">
         <f>SUM(G16:BJ16)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E16" s="50"/>
       <c r="F16" s="51"/>
@@ -3251,7 +3253,9 @@
       <c r="J16" s="55">
         <v>3</v>
       </c>
-      <c r="K16" s="63"/>
+      <c r="K16" s="63">
+        <v>3</v>
+      </c>
       <c r="L16" s="57"/>
       <c r="M16" s="58"/>
       <c r="N16" s="59"/>
@@ -3386,7 +3390,7 @@
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -3532,7 +3536,7 @@
       </c>
       <c r="D20" s="83">
         <f t="shared" ref="D20:D30" si="0">SUM(G20:BJ20)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E20" s="50"/>
       <c r="F20" s="51"/>
@@ -3540,7 +3544,9 @@
       <c r="H20" s="60"/>
       <c r="I20" s="55"/>
       <c r="J20" s="55"/>
-      <c r="K20" s="56"/>
+      <c r="K20" s="56">
+        <v>4</v>
+      </c>
       <c r="L20" s="57"/>
       <c r="M20" s="58"/>
       <c r="N20" s="59"/>
@@ -5189,7 +5195,7 @@
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5211,7 +5217,7 @@
       </c>
       <c r="K43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L43" s="39">
         <f t="shared" si="3"/>
@@ -5487,7 +5493,7 @@
       </c>
       <c r="D3" s="80">
         <f>Zeitplanung!D9</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3" s="82"/>
       <c r="F3" s="81"/>
@@ -5504,7 +5510,7 @@
       </c>
       <c r="D4" s="80">
         <f>Zeitplanung!D14</f>
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E4" s="82"/>
       <c r="F4" s="81"/>
@@ -5521,7 +5527,7 @@
       </c>
       <c r="D5" s="80">
         <f>Zeitplanung!D18</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E5" s="82"/>
       <c r="F5" s="81"/>

</xml_diff>

<commit_message>
Priorität nachgetragen und Anfgefangen mit Funktionen
</commit_message>
<xml_diff>
--- a/doc/Zeitplanung.xlsx
+++ b/doc/Zeitplanung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nick_privat\FlappyExtremeProject\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{545EAEA5-074D-4DEB-AD75-545F9FFA590A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5756FA9B-6DA4-4B26-ABB0-E002C4061669}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2107,8 +2107,8 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -3166,7 +3166,9 @@
         <f>SUM(G15:BJ15)</f>
         <v>8</v>
       </c>
-      <c r="E15" s="50"/>
+      <c r="E15" s="50">
+        <v>1</v>
+      </c>
       <c r="F15" s="89" t="s">
         <v>46</v>
       </c>
@@ -3245,7 +3247,9 @@
         <f>SUM(G16:BJ16)</f>
         <v>6</v>
       </c>
-      <c r="E16" s="50"/>
+      <c r="E16" s="50">
+        <v>1</v>
+      </c>
       <c r="F16" s="51"/>
       <c r="G16" s="59"/>
       <c r="H16" s="60"/>
@@ -3465,7 +3469,9 @@
         <f>SUM(G19:BJ19)</f>
         <v>0</v>
       </c>
-      <c r="E19" s="50"/>
+      <c r="E19" s="50">
+        <v>1</v>
+      </c>
       <c r="F19" s="51"/>
       <c r="G19" s="53"/>
       <c r="H19" s="54"/>
@@ -3538,7 +3544,9 @@
         <f t="shared" ref="D20:D30" si="0">SUM(G20:BJ20)</f>
         <v>4</v>
       </c>
-      <c r="E20" s="50"/>
+      <c r="E20" s="50">
+        <v>1</v>
+      </c>
       <c r="F20" s="51"/>
       <c r="G20" s="59"/>
       <c r="H20" s="60"/>
@@ -3613,7 +3621,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E21" s="50"/>
+      <c r="E21" s="50">
+        <v>1</v>
+      </c>
       <c r="F21" s="52">
         <v>21.12</v>
       </c>
@@ -3688,7 +3698,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E22" s="50"/>
+      <c r="E22" s="50">
+        <v>1</v>
+      </c>
       <c r="F22" s="51" t="s">
         <v>57</v>
       </c>
@@ -3763,7 +3775,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E23" s="50"/>
+      <c r="E23" s="50">
+        <v>2</v>
+      </c>
       <c r="F23" s="51" t="s">
         <v>57</v>
       </c>
@@ -3838,7 +3852,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E24" s="50"/>
+      <c r="E24" s="50">
+        <v>2</v>
+      </c>
       <c r="F24" s="51"/>
       <c r="G24" s="59"/>
       <c r="H24" s="60"/>
@@ -3911,7 +3927,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E25" s="50"/>
+      <c r="E25" s="50">
+        <v>2</v>
+      </c>
       <c r="F25" s="51"/>
       <c r="G25" s="59"/>
       <c r="H25" s="60"/>
@@ -3984,7 +4002,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E26" s="50"/>
+      <c r="E26" s="50">
+        <v>3</v>
+      </c>
       <c r="F26" s="51"/>
       <c r="G26" s="59"/>
       <c r="H26" s="60"/>
@@ -4407,7 +4427,9 @@
         <f>SUM(G32:BJ32)</f>
         <v>0</v>
       </c>
-      <c r="E32" s="50"/>
+      <c r="E32" s="50">
+        <v>1</v>
+      </c>
       <c r="F32" s="51"/>
       <c r="G32" s="53"/>
       <c r="H32" s="54"/>
@@ -4480,7 +4502,9 @@
         <f t="shared" ref="D33:D35" si="1">SUM(G33:BJ33)</f>
         <v>0</v>
       </c>
-      <c r="E33" s="50"/>
+      <c r="E33" s="50">
+        <v>1</v>
+      </c>
       <c r="F33" s="51"/>
       <c r="G33" s="59"/>
       <c r="H33" s="60"/>
@@ -4553,7 +4577,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E34" s="50"/>
+      <c r="E34" s="50">
+        <v>1</v>
+      </c>
       <c r="F34" s="51"/>
       <c r="G34" s="59"/>
       <c r="H34" s="60"/>

</xml_diff>

<commit_message>
1 Version coin System und Zeit von Freitag nachgetragen
</commit_message>
<xml_diff>
--- a/doc/Zeitplanung.xlsx
+++ b/doc/Zeitplanung.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="DieseArbeitsmappe" showPivotChartFilter="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\FlappyExtremeProject\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\TheFlappyExtreme\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AEC4784D-5F09-4091-8E1B-D0374E1B7358}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2E6DBE3B-1C25-475B-A995-7A6B6B2D879B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8376" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1594,13 +1594,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2107,8 +2107,8 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -2709,7 +2709,7 @@
       </c>
       <c r="D9" s="42">
         <f>SUM(D10:D13)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E9" s="32"/>
       <c r="F9" s="31"/>
@@ -2939,7 +2939,7 @@
       </c>
       <c r="D12" s="83">
         <f>SUM(G12:BJ12)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" s="50">
         <v>1</v>
@@ -2958,7 +2958,9 @@
       <c r="O12" s="60"/>
       <c r="P12" s="61"/>
       <c r="Q12" s="61"/>
-      <c r="R12" s="63"/>
+      <c r="R12" s="63">
+        <v>1</v>
+      </c>
       <c r="S12" s="57"/>
       <c r="T12" s="58"/>
       <c r="U12" s="59"/>
@@ -3396,7 +3398,7 @@
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -3625,7 +3627,7 @@
       </c>
       <c r="D21" s="83">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E21" s="50">
         <v>1</v>
@@ -3648,7 +3650,9 @@
       <c r="Q21" s="63">
         <v>4</v>
       </c>
-      <c r="R21" s="63"/>
+      <c r="R21" s="63">
+        <v>3</v>
+      </c>
       <c r="S21" s="57"/>
       <c r="T21" s="58"/>
       <c r="U21" s="59"/>
@@ -3706,7 +3710,7 @@
       </c>
       <c r="D22" s="83">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E22" s="50">
         <v>1</v>
@@ -3727,7 +3731,9 @@
       <c r="Q22" s="55">
         <v>4</v>
       </c>
-      <c r="R22" s="56"/>
+      <c r="R22" s="56">
+        <v>3</v>
+      </c>
       <c r="S22" s="57"/>
       <c r="T22" s="58"/>
       <c r="U22" s="59"/>
@@ -3785,7 +3791,7 @@
       </c>
       <c r="D23" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="50">
         <v>2</v>
@@ -3804,7 +3810,9 @@
       <c r="O23" s="60"/>
       <c r="P23" s="61"/>
       <c r="Q23" s="61"/>
-      <c r="R23" s="56"/>
+      <c r="R23" s="56">
+        <v>1</v>
+      </c>
       <c r="S23" s="57"/>
       <c r="T23" s="58"/>
       <c r="U23" s="59"/>
@@ -5233,7 +5241,7 @@
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5283,7 +5291,7 @@
       </c>
       <c r="R43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="S43" s="39">
         <f t="shared" si="3"/>
@@ -5531,7 +5539,7 @@
       </c>
       <c r="D3" s="80">
         <f>Zeitplanung!D9</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E3" s="82"/>
       <c r="F3" s="81"/>
@@ -5565,7 +5573,7 @@
       </c>
       <c r="D5" s="80">
         <f>Zeitplanung!D18</f>
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="E5" s="82"/>
       <c r="F5" s="81"/>

</xml_diff>

<commit_message>
Beim Game Over screen werden jetzt erreichte Punktzahl und Coins angezeigt.
</commit_message>
<xml_diff>
--- a/doc/Zeitplanung.xlsx
+++ b/doc/Zeitplanung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\TheFlappyExtreme\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DC4F704D-1178-4C11-A57F-2A391430E989}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4E7F9043-68C4-4BFA-BE1C-58997FF0CFEB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8376" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1600,7 +1600,7 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>49</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2107,8 +2107,8 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="Y22" sqref="Y22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AT22" sqref="AT22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -3400,7 +3400,7 @@
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -3714,7 +3714,7 @@
       </c>
       <c r="D22" s="83">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="E22" s="50">
         <v>1</v>
@@ -3769,7 +3769,9 @@
       <c r="AO22" s="58"/>
       <c r="AP22" s="59"/>
       <c r="AQ22" s="60"/>
-      <c r="AR22" s="87"/>
+      <c r="AR22" s="87">
+        <v>8</v>
+      </c>
       <c r="AS22" s="55"/>
       <c r="AT22" s="56"/>
       <c r="AU22" s="57"/>
@@ -5255,7 +5257,7 @@
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5409,7 +5411,7 @@
       </c>
       <c r="AR43" s="39">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AS43" s="39">
         <f t="shared" si="4"/>
@@ -5587,7 +5589,7 @@
       </c>
       <c r="D5" s="80">
         <f>Zeitplanung!D18</f>
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E5" s="82"/>
       <c r="F5" s="81"/>

</xml_diff>